<commit_message>
edit database and validate import excel
</commit_message>
<xml_diff>
--- a/public/files/template.xlsx
+++ b/public/files/template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Teacher</t>
   </si>
@@ -53,15 +53,6 @@
     <t>2nd Semester</t>
   </si>
   <si>
-    <t>Grade Average</t>
-  </si>
-  <si>
-    <t>Year Grade</t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
     <t>Student Name</t>
   </si>
   <si>
@@ -89,17 +80,37 @@
     <t>Sem 2</t>
   </si>
   <si>
-    <t>##</t>
+    <t>Thai</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>M12ff@</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -122,13 +133,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -407,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -418,7 +432,7 @@
     <col min="2" max="2" width="19.796875" customWidth="1"/>
     <col min="3" max="3" width="11.09765625" customWidth="1"/>
     <col min="4" max="4" width="11.69921875" customWidth="1"/>
-    <col min="11" max="11" width="14.59765625" customWidth="1"/>
+    <col min="11" max="11" width="10.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -433,6 +447,9 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
@@ -441,6 +458,9 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
@@ -456,48 +476,68 @@
         <v>8</v>
       </c>
       <c r="K4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="L4" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
+      <c r="H5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" t="s">
+      <c r="I5" t="s">
         <v>16</v>
       </c>
-      <c r="G5" t="s">
+      <c r="J5" t="s">
         <v>17</v>
       </c>
-      <c r="H5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>19</v>
       </c>
-      <c r="J5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" t="s">
-        <v>11</v>
-      </c>
       <c r="L5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6">
+        <v>1.5555000000000001</v>
+      </c>
+      <c r="D6" t="s">
         <v>21</v>
+      </c>
+      <c r="E6">
+        <v>1.2</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>